<commit_message>
Mediciones realizadas, ademas armé una placa chica con dos level shifter PNP vs MOSFET, comparandolo en dos mediciones sencillas. Informe, ready to go!
</commit_message>
<xml_diff>
--- a/EJ5/Mediciones/Mediciones.xlsx
+++ b/EJ5/Mediciones/Mediciones.xlsx
@@ -9,7 +9,7 @@
     </mc:Choice>
   </mc:AlternateContent>
   <bookViews>
-    <workbookView xWindow="0" yWindow="0" windowWidth="20490" windowHeight="7620" activeTab="1"/>
+    <workbookView xWindow="0" yWindow="0" windowWidth="20490" windowHeight="7620"/>
   </bookViews>
   <sheets>
     <sheet name="Ensayos 1° Circuito" sheetId="1" r:id="rId1"/>
@@ -25,7 +25,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="65" uniqueCount="34">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="68" uniqueCount="37">
   <si>
     <t>Estados</t>
   </si>
@@ -166,6 +166,15 @@
   </si>
   <si>
     <t>Simulando cargas capacitivas por más compuertas CMOS, los transitorios crecerían y deberían haber problemas por niveles de tensión. Medir entrada, salida y señales.</t>
+  </si>
+  <si>
+    <t>Entrada es la señal amarilla, la salida es la verde.</t>
+  </si>
+  <si>
+    <t>Probe con una señal cuadrada, y no pasó nada. Con ninguna frecuencia ninguna anomalía, salvo por los tiempos de propagación. Se me ocurrió probar con una señal triangular, se observa una anomalía, porque tiene que superar dos veces el nivel de tensión.</t>
+  </si>
+  <si>
+    <t>Señal amarilla es la entrada cuadrada, la verde es la salida y luego la morada corresponde a la señal intermedia entre la AND y la OR. Se miden diferentes escenarios sin carga y con carga variando.</t>
   </si>
 </sst>
 </file>
@@ -444,35 +453,35 @@
     <xf numFmtId="0" fontId="0" fillId="2" borderId="12" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" vertical="center" wrapText="1"/>
     </xf>
+    <xf numFmtId="0" fontId="0" fillId="2" borderId="11" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="2" borderId="13" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="4" borderId="7" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="3" borderId="8" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="3" borderId="9" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="3" borderId="10" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="2" borderId="7" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="2" borderId="7" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
     <xf numFmtId="0" fontId="3" fillId="5" borderId="4" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
     <xf numFmtId="0" fontId="3" fillId="5" borderId="6" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="2" borderId="11" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="2" borderId="13" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="4" borderId="7" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="3" borderId="8" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="3" borderId="9" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="3" borderId="10" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="2" borderId="7" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="2" borderId="7" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
     <xf numFmtId="0" fontId="4" fillId="5" borderId="4" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
@@ -487,14 +496,7 @@
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
   </cellStyles>
-  <dxfs count="6">
-    <dxf>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FF00B050"/>
-        </patternFill>
-      </fill>
-    </dxf>
+  <dxfs count="4">
     <dxf>
       <fill>
         <patternFill>
@@ -506,13 +508,6 @@
       <fill>
         <patternFill>
           <bgColor rgb="FF00B050"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FFFF0000"/>
         </patternFill>
       </fill>
     </dxf>
@@ -808,8 +803,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="B1:U12"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="B12" sqref="B12:C12"/>
+    <sheetView tabSelected="1" zoomScale="85" zoomScaleNormal="85" workbookViewId="0">
+      <selection activeCell="B13" sqref="B13"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -845,109 +840,111 @@
       </c>
       <c r="U2" s="2"/>
     </row>
-    <row r="3" spans="2:21" x14ac:dyDescent="0.25">
-      <c r="B3" s="17" t="s">
+    <row r="3" spans="2:21" ht="30" x14ac:dyDescent="0.25">
+      <c r="B3" s="15" t="s">
         <v>11</v>
       </c>
       <c r="C3" s="8" t="s">
         <v>13</v>
       </c>
-      <c r="D3" s="11" t="s">
+      <c r="D3" s="9" t="s">
         <v>21</v>
       </c>
-      <c r="E3" s="13" t="s">
-        <v>2</v>
-      </c>
-      <c r="F3" s="12"/>
+      <c r="E3" s="11" t="s">
+        <v>5</v>
+      </c>
+      <c r="F3" s="10" t="s">
+        <v>34</v>
+      </c>
       <c r="U3" s="2" t="s">
         <v>1</v>
       </c>
     </row>
     <row r="4" spans="2:21" x14ac:dyDescent="0.25">
-      <c r="B4" s="17" t="s">
+      <c r="B4" s="15" t="s">
         <v>12</v>
       </c>
       <c r="C4" s="8" t="s">
         <v>14</v>
       </c>
-      <c r="D4" s="11" t="s">
+      <c r="D4" s="9" t="s">
         <v>21</v>
       </c>
-      <c r="E4" s="13" t="s">
-        <v>2</v>
-      </c>
-      <c r="F4" s="12"/>
+      <c r="E4" s="11" t="s">
+        <v>5</v>
+      </c>
+      <c r="F4" s="10"/>
       <c r="U4" s="2" t="s">
         <v>2</v>
       </c>
     </row>
     <row r="5" spans="2:21" x14ac:dyDescent="0.25">
-      <c r="B5" s="17" t="s">
+      <c r="B5" s="15" t="s">
         <v>15</v>
       </c>
       <c r="C5" s="8" t="s">
         <v>13</v>
       </c>
-      <c r="D5" s="11" t="s">
+      <c r="D5" s="9" t="s">
         <v>21</v>
       </c>
-      <c r="E5" s="13" t="s">
-        <v>2</v>
-      </c>
-      <c r="F5" s="12"/>
+      <c r="E5" s="11" t="s">
+        <v>5</v>
+      </c>
+      <c r="F5" s="10"/>
       <c r="U5" s="2" t="s">
         <v>3</v>
       </c>
     </row>
     <row r="6" spans="2:21" x14ac:dyDescent="0.25">
-      <c r="B6" s="17" t="s">
+      <c r="B6" s="15" t="s">
         <v>16</v>
       </c>
       <c r="C6" s="8" t="s">
         <v>14</v>
       </c>
-      <c r="D6" s="11" t="s">
+      <c r="D6" s="9" t="s">
         <v>21</v>
       </c>
-      <c r="E6" s="13" t="s">
-        <v>2</v>
-      </c>
-      <c r="F6" s="12"/>
+      <c r="E6" s="11" t="s">
+        <v>5</v>
+      </c>
+      <c r="F6" s="10"/>
       <c r="U6" s="2" t="s">
         <v>4</v>
       </c>
     </row>
     <row r="7" spans="2:21" ht="30.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="B7" s="17" t="s">
+      <c r="B7" s="15" t="s">
         <v>18</v>
       </c>
       <c r="C7" s="7" t="s">
         <v>19</v>
       </c>
-      <c r="D7" s="11" t="s">
+      <c r="D7" s="9" t="s">
         <v>21</v>
       </c>
-      <c r="E7" s="13" t="s">
-        <v>2</v>
-      </c>
-      <c r="F7" s="12"/>
+      <c r="E7" s="11" t="s">
+        <v>5</v>
+      </c>
+      <c r="F7" s="10"/>
       <c r="U7" s="3" t="s">
         <v>5</v>
       </c>
     </row>
     <row r="9" spans="2:21" ht="15.75" thickBot="1" x14ac:dyDescent="0.3"/>
     <row r="10" spans="2:21" ht="24" thickBot="1" x14ac:dyDescent="0.4">
-      <c r="B10" s="9" t="s">
+      <c r="B10" s="17" t="s">
         <v>17</v>
       </c>
-      <c r="C10" s="10"/>
+      <c r="C10" s="18"/>
     </row>
     <row r="11" spans="2:21" ht="15.75" thickBot="1" x14ac:dyDescent="0.3"/>
     <row r="12" spans="2:21" ht="24" thickBot="1" x14ac:dyDescent="0.4">
-      <c r="B12" s="9" t="s">
+      <c r="B12" s="17" t="s">
         <v>20</v>
       </c>
-      <c r="C12" s="10"/>
+      <c r="C12" s="18"/>
     </row>
   </sheetData>
   <mergeCells count="2">
@@ -999,8 +996,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="B1:U10"/>
   <sheetViews>
-    <sheetView tabSelected="1" zoomScale="85" zoomScaleNormal="85" workbookViewId="0">
-      <selection activeCell="B12" sqref="B12"/>
+    <sheetView zoomScale="70" zoomScaleNormal="70" workbookViewId="0">
+      <selection activeCell="B13" sqref="B13"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -1021,109 +1018,113 @@
       </c>
     </row>
     <row r="2" spans="2:21" x14ac:dyDescent="0.25">
-      <c r="B2" s="14" t="s">
+      <c r="B2" s="12" t="s">
         <v>6</v>
       </c>
-      <c r="C2" s="15" t="s">
+      <c r="C2" s="13" t="s">
         <v>7</v>
       </c>
-      <c r="D2" s="16" t="s">
+      <c r="D2" s="14" t="s">
         <v>8</v>
       </c>
-      <c r="E2" s="15" t="s">
+      <c r="E2" s="13" t="s">
         <v>9</v>
       </c>
-      <c r="F2" s="15" t="s">
+      <c r="F2" s="13" t="s">
         <v>10</v>
       </c>
       <c r="U2" s="2"/>
     </row>
     <row r="3" spans="2:21" ht="30" x14ac:dyDescent="0.25">
-      <c r="B3" s="18" t="s">
+      <c r="B3" s="16" t="s">
         <v>22</v>
       </c>
       <c r="C3" s="8" t="s">
         <v>26</v>
       </c>
-      <c r="D3" s="11" t="s">
+      <c r="D3" s="9" t="s">
         <v>27</v>
       </c>
-      <c r="E3" s="13" t="s">
-        <v>2</v>
-      </c>
-      <c r="F3" s="12"/>
+      <c r="E3" s="11" t="s">
+        <v>5</v>
+      </c>
+      <c r="F3" s="10"/>
       <c r="U3" s="2" t="s">
         <v>1</v>
       </c>
     </row>
-    <row r="4" spans="2:21" ht="45" x14ac:dyDescent="0.25">
-      <c r="B4" s="18" t="s">
+    <row r="4" spans="2:21" ht="60" x14ac:dyDescent="0.25">
+      <c r="B4" s="16" t="s">
         <v>23</v>
       </c>
       <c r="C4" s="8" t="s">
         <v>28</v>
       </c>
-      <c r="D4" s="11" t="s">
+      <c r="D4" s="9" t="s">
         <v>27</v>
       </c>
-      <c r="E4" s="13" t="s">
-        <v>2</v>
-      </c>
-      <c r="F4" s="12"/>
+      <c r="E4" s="11" t="s">
+        <v>5</v>
+      </c>
+      <c r="F4" s="10" t="s">
+        <v>35</v>
+      </c>
       <c r="U4" s="2" t="s">
         <v>2</v>
       </c>
     </row>
     <row r="5" spans="2:21" ht="45" x14ac:dyDescent="0.25">
-      <c r="B5" s="18" t="s">
+      <c r="B5" s="16" t="s">
         <v>24</v>
       </c>
       <c r="C5" s="8" t="s">
         <v>29</v>
       </c>
-      <c r="D5" s="11" t="s">
+      <c r="D5" s="9" t="s">
         <v>27</v>
       </c>
-      <c r="E5" s="13" t="s">
-        <v>2</v>
-      </c>
-      <c r="F5" s="12"/>
+      <c r="E5" s="11" t="s">
+        <v>5</v>
+      </c>
+      <c r="F5" s="10" t="s">
+        <v>36</v>
+      </c>
       <c r="U5" s="2" t="s">
         <v>3</v>
       </c>
     </row>
     <row r="6" spans="2:21" ht="30" x14ac:dyDescent="0.25">
-      <c r="B6" s="18" t="s">
+      <c r="B6" s="16" t="s">
         <v>25</v>
       </c>
       <c r="C6" s="8" t="s">
         <v>30</v>
       </c>
-      <c r="D6" s="11" t="s">
+      <c r="D6" s="9" t="s">
         <v>27</v>
       </c>
-      <c r="E6" s="13" t="s">
-        <v>2</v>
-      </c>
-      <c r="F6" s="12"/>
+      <c r="E6" s="11" t="s">
+        <v>5</v>
+      </c>
+      <c r="F6" s="10"/>
       <c r="U6" s="2" t="s">
         <v>4</v>
       </c>
     </row>
     <row r="7" spans="2:21" ht="30.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="B7" s="18" t="s">
+      <c r="B7" s="16" t="s">
         <v>32</v>
       </c>
       <c r="C7" s="8" t="s">
         <v>33</v>
       </c>
-      <c r="D7" s="11" t="s">
+      <c r="D7" s="9" t="s">
         <v>27</v>
       </c>
-      <c r="E7" s="13" t="s">
-        <v>2</v>
-      </c>
-      <c r="F7" s="12"/>
+      <c r="E7" s="11" t="s">
+        <v>5</v>
+      </c>
+      <c r="F7" s="10"/>
       <c r="U7" s="3" t="s">
         <v>5</v>
       </c>

</xml_diff>